<commit_message>
Implemented cell formatting. Just need to figure out how to format the cell widths and improve overall time complexity.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -16,8 +16,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,16 +29,59 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -42,12 +89,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,71 +536,93 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>FY23-24 LEAP Spring '24</t>
         </is>
       </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Summary of Key Financial Metrics for the LDI Financial Forecast Spreadsheet</t>
         </is>
       </c>
+      <c r="B2" s="3" t="n"/>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="3" t="n"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
+      <c r="H2" s="3" t="n"/>
+      <c r="I2" s="3" t="n"/>
+      <c r="J2" s="3" t="n"/>
+      <c r="K2" s="3" t="n"/>
+      <c r="L2" s="3" t="n"/>
     </row>
     <row r="3">
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr">
         <is>
           <t># of Students</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="5" t="inlineStr">
         <is>
           <t>Price ($)/Student</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="4" t="inlineStr">
         <is>
           <t>Revenue</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="4" t="inlineStr">
         <is>
           <t>Gross Profit</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="4" t="inlineStr">
         <is>
           <t>LDI Overhead</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="4" t="inlineStr">
         <is>
           <t>EBITA</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="4" t="inlineStr">
         <is>
           <t>SIA</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="4" t="inlineStr">
         <is>
           <t>G&amp;A</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" s="4" t="inlineStr">
         <is>
           <t>Net Profit</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L3" s="4" t="inlineStr">
         <is>
           <t>Margin</t>
         </is>
@@ -496,255 +632,293 @@
       <c r="B4" t="n">
         <v>40</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="6" t="n">
         <v>2045</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="7" t="n">
         <v>95000</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="8" t="n">
         <v>18976.2</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" s="8" t="n">
         <v>76023.8</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" s="8" t="n">
         <v>38000</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4" s="8" t="n">
         <v>38023.8</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="8" t="n">
         <v>19428.8842</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4" s="8" t="n">
         <v>3468.79082268</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4" s="8" t="n">
         <v>15126.12497732</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4" s="9" t="n">
         <v>0.1592223681823158</v>
       </c>
     </row>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>FY23-24 KAIST FINANCE 2024</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="2" t="n"/>
+      <c r="K8" s="2" t="n"/>
+      <c r="L8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Summary of Key Financial Metrics for the LDI Financial Forecast Spreadsheet</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="3" t="n"/>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="3" t="n"/>
+      <c r="E9" s="3" t="n"/>
+      <c r="F9" s="3" t="n"/>
+      <c r="G9" s="3" t="n"/>
+      <c r="H9" s="3" t="n"/>
+      <c r="I9" s="3" t="n"/>
+      <c r="J9" s="3" t="n"/>
+      <c r="K9" s="3" t="n"/>
+      <c r="L9" s="3" t="n"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="10" t="inlineStr">
         <is>
           <t># of Students</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>Price ($)/Student</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D10" s="10" t="inlineStr">
         <is>
           <t>Revenue</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" s="10" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F10" s="10" t="inlineStr">
         <is>
           <t>Gross Profit</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G10" s="10" t="inlineStr">
         <is>
           <t>LDI Overhead</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H10" s="10" t="inlineStr">
         <is>
           <t>EBITA</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I10" s="10" t="inlineStr">
         <is>
           <t>SIA</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="J10" s="10" t="inlineStr">
         <is>
           <t>G&amp;A</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="K10" s="10" t="inlineStr">
         <is>
           <t>Net Profit</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="L10" s="10" t="inlineStr">
         <is>
           <t>Margin</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" t="n">
+    <row r="11">
+      <c r="B11" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C11" s="13" t="n">
         <v>22000</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" s="14" t="n">
         <v>220000</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E11" s="14" t="n">
         <v>63750</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F11" s="14" t="n">
         <v>156250</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G11" s="14" t="n">
         <v>66000</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H11" s="14" t="n">
         <v>90250</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I11" s="14" t="n">
         <v>44244.75</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J11" s="14" t="n">
         <v>5890.650000000001</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K11" s="14" t="n">
         <v>40114.6</v>
       </c>
-      <c r="L10" t="n">
+      <c r="L11" s="15" t="n">
         <v>0.1823390909090909</v>
       </c>
     </row>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>FY23-24 Q1-Q2 KAIST GLP Summer-Fall '23</t>
         </is>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="n"/>
+      <c r="H15" s="2" t="n"/>
+      <c r="I15" s="2" t="n"/>
+      <c r="J15" s="2" t="n"/>
+      <c r="K15" s="2" t="n"/>
+      <c r="L15" s="2" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
         <is>
           <t>Summary of Key Financial Metrics for the LDI Financial Forecast Spreadsheet</t>
         </is>
       </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="inlineStr">
+      <c r="B16" s="3" t="n"/>
+      <c r="C16" s="3" t="n"/>
+      <c r="D16" s="3" t="n"/>
+      <c r="E16" s="3" t="n"/>
+      <c r="F16" s="3" t="n"/>
+      <c r="G16" s="3" t="n"/>
+      <c r="H16" s="3" t="n"/>
+      <c r="I16" s="3" t="n"/>
+      <c r="J16" s="3" t="n"/>
+      <c r="K16" s="3" t="n"/>
+      <c r="L16" s="3" t="n"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="4" t="inlineStr">
         <is>
           <t># of Students</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C17" s="5" t="inlineStr">
         <is>
           <t>Price ($)/Student</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D17" s="4" t="inlineStr">
         <is>
           <t>Revenue</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E17" s="4" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F17" s="4" t="inlineStr">
         <is>
           <t>Gross Profit</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G17" s="4" t="inlineStr">
         <is>
           <t>LDI Overhead</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H17" s="4" t="inlineStr">
         <is>
           <t>EBITA</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I17" s="4" t="inlineStr">
         <is>
           <t>SIA</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J17" s="4" t="inlineStr">
         <is>
           <t>G&amp;A</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="K17" s="4" t="inlineStr">
         <is>
           <t>Net Profit</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="L17" s="4" t="inlineStr">
         <is>
           <t>Margin</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" t="n">
+    <row r="18">
+      <c r="B18" t="n">
         <v>14</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C18" s="6" t="n">
         <v>14171.77</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D18" s="7" t="n">
         <v>268684.78</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E18" s="8" t="n">
         <v>39588</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F18" s="8" t="n">
         <v>229096.78</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G18" s="8" t="n">
         <v>107473.912</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H18" s="8" t="n">
         <v>121622.868</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I18" s="8" t="n">
         <v>50148.11199200001</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J18" s="8" t="n">
         <v>8361.705017260801</v>
       </c>
-      <c r="K16" t="n">
+      <c r="K18" s="8" t="n">
         <v>63113.05099073921</v>
       </c>
-      <c r="L16" t="n">
+      <c r="L18" s="9" t="n">
         <v>0.2348962639072418</v>
       </c>
     </row>
-    <row r="17"/>
-    <row r="18"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Figured out the column width formatting
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -534,6 +534,20 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">

</xml_diff>